<commit_message>
Fixed Rota DT Old Values Not Overwritten
</commit_message>
<xml_diff>
--- a/examples/rota_dt/spreadsheets/KS3 Jan rotations COLOUR Art & DT TT 2024.xlsx
+++ b/examples/rota_dt/spreadsheets/KS3 Jan rotations COLOUR Art & DT TT 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\examples\rota_dt\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F07A497-1A55-4FCF-9831-901A7C0C57AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECECEB5C-FA9D-4666-A63B-C83B665BD952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD7A2D35-DBA8-481B-A8FB-700A037D20F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DD7A2D35-DBA8-481B-A8FB-700A037D20F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="2" r:id="rId1"/>
@@ -1623,16 +1623,70 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1640,60 +1694,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2011,7 +2011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A503ABD-6187-4903-A0A0-8797012A8480}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -2773,9 +2773,9 @@
   </sheetPr>
   <dimension ref="A1:BT16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="AK1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AG1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BU1" sqref="BU1"/>
+      <selection pane="bottomLeft" activeCell="AM10" sqref="AM10:AN10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2799,219 +2799,219 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120" t="s">
+      <c r="C1" s="97"/>
+      <c r="D1" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120" t="s">
+      <c r="E1" s="97"/>
+      <c r="F1" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120" t="s">
+      <c r="G1" s="97"/>
+      <c r="H1" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120" t="s">
+      <c r="I1" s="97"/>
+      <c r="J1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120" t="s">
+      <c r="K1" s="97"/>
+      <c r="L1" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120" t="s">
+      <c r="M1" s="97"/>
+      <c r="N1" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120" t="s">
+      <c r="O1" s="97"/>
+      <c r="P1" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="120"/>
-      <c r="R1" s="120"/>
-      <c r="S1" s="120" t="s">
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120" t="s">
+      <c r="T1" s="97"/>
+      <c r="U1" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120" t="s">
+      <c r="V1" s="97"/>
+      <c r="W1" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120" t="s">
+      <c r="X1" s="97"/>
+      <c r="Y1" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="120"/>
-      <c r="AA1" s="120" t="s">
+      <c r="Z1" s="97"/>
+      <c r="AA1" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="120"/>
-      <c r="AC1" s="120" t="s">
+      <c r="AB1" s="97"/>
+      <c r="AC1" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="120"/>
-      <c r="AE1" s="120" t="s">
+      <c r="AD1" s="97"/>
+      <c r="AE1" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="120"/>
-      <c r="AG1" s="120" t="s">
+      <c r="AF1" s="97"/>
+      <c r="AG1" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="120"/>
-      <c r="AI1" s="120" t="s">
+      <c r="AH1" s="97"/>
+      <c r="AI1" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="AJ1" s="120"/>
-      <c r="AK1" s="120" t="s">
+      <c r="AJ1" s="97"/>
+      <c r="AK1" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="AL1" s="120"/>
-      <c r="AM1" s="120" t="s">
+      <c r="AL1" s="97"/>
+      <c r="AM1" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="AN1" s="120"/>
-      <c r="AO1" s="120" t="s">
+      <c r="AN1" s="97"/>
+      <c r="AO1" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="AP1" s="120"/>
-      <c r="AQ1" s="120" t="s">
+      <c r="AP1" s="97"/>
+      <c r="AQ1" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="AR1" s="120"/>
-      <c r="AS1" s="120" t="s">
+      <c r="AR1" s="97"/>
+      <c r="AS1" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="AT1" s="120"/>
-      <c r="AU1" s="120" t="s">
+      <c r="AT1" s="97"/>
+      <c r="AU1" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="AV1" s="120"/>
-      <c r="AW1" s="120" t="s">
+      <c r="AV1" s="97"/>
+      <c r="AW1" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="AX1" s="120"/>
-      <c r="AY1" s="120" t="s">
+      <c r="AX1" s="97"/>
+      <c r="AY1" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="AZ1" s="120"/>
-      <c r="BA1" s="120" t="s">
+      <c r="AZ1" s="97"/>
+      <c r="BA1" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="BB1" s="120"/>
-      <c r="BC1" s="120" t="s">
+      <c r="BB1" s="97"/>
+      <c r="BC1" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="BD1" s="120"/>
-      <c r="BE1" s="120" t="s">
+      <c r="BD1" s="97"/>
+      <c r="BE1" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="BF1" s="120"/>
-      <c r="BG1" s="120" t="s">
+      <c r="BF1" s="97"/>
+      <c r="BG1" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="BH1" s="120"/>
-      <c r="BI1" s="120" t="s">
+      <c r="BH1" s="97"/>
+      <c r="BI1" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="BJ1" s="120"/>
-      <c r="BK1" s="120" t="s">
+      <c r="BJ1" s="97"/>
+      <c r="BK1" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="BL1" s="120"/>
-      <c r="BM1" s="120" t="s">
+      <c r="BL1" s="97"/>
+      <c r="BM1" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="BN1" s="120"/>
-      <c r="BO1" s="120" t="s">
+      <c r="BN1" s="97"/>
+      <c r="BO1" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="BP1" s="120"/>
-      <c r="BQ1" s="120" t="s">
+      <c r="BP1" s="97"/>
+      <c r="BQ1" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="BR1" s="120"/>
-      <c r="BS1" s="120" t="s">
+      <c r="BR1" s="97"/>
+      <c r="BS1" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="BT1" s="120"/>
+      <c r="BT1" s="97"/>
     </row>
     <row r="2" spans="1:72" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="99" t="s">
+      <c r="B2" s="99"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="100"/>
-      <c r="F2" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="114"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="100"/>
       <c r="H2" s="103" t="s">
         <v>38</v>
       </c>
       <c r="I2" s="104"/>
-      <c r="J2" s="113" t="s">
+      <c r="J2" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="114"/>
-      <c r="L2" s="99" t="s">
+      <c r="K2" s="100"/>
+      <c r="L2" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="100"/>
-      <c r="N2" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="98"/>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="98"/>
-      <c r="S2" s="113" t="s">
+      <c r="M2" s="102"/>
+      <c r="N2" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="106"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="114"/>
-      <c r="U2" s="99" t="s">
+      <c r="T2" s="100"/>
+      <c r="U2" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="V2" s="100"/>
-      <c r="W2" s="99" t="s">
+      <c r="V2" s="102"/>
+      <c r="W2" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="100"/>
-      <c r="Y2" s="113" t="s">
+      <c r="X2" s="102"/>
+      <c r="Y2" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="Z2" s="114"/>
+      <c r="Z2" s="100"/>
       <c r="AA2" s="103" t="s">
         <v>45</v>
       </c>
       <c r="AB2" s="104"/>
-      <c r="AC2" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="98"/>
-      <c r="AE2" s="97"/>
-      <c r="AF2" s="98"/>
-      <c r="AG2" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="98"/>
+      <c r="AC2" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="106"/>
+      <c r="AE2" s="105"/>
+      <c r="AF2" s="106"/>
+      <c r="AG2" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="106"/>
       <c r="AI2" s="103" t="s">
         <v>40</v>
       </c>
       <c r="AJ2" s="104"/>
-      <c r="AK2" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="98"/>
+      <c r="AK2" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="106"/>
       <c r="AM2" s="107" t="s">
         <v>46</v>
       </c>
@@ -3020,65 +3020,65 @@
         <v>38</v>
       </c>
       <c r="AP2" s="104"/>
-      <c r="AQ2" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="114"/>
-      <c r="AS2" s="113"/>
-      <c r="AT2" s="114"/>
-      <c r="AU2" s="99" t="s">
+      <c r="AQ2" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="100"/>
+      <c r="AS2" s="99"/>
+      <c r="AT2" s="100"/>
+      <c r="AU2" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="AV2" s="100"/>
-      <c r="AW2" s="113" t="s">
+      <c r="AV2" s="102"/>
+      <c r="AW2" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="AX2" s="114"/>
-      <c r="AY2" s="99" t="s">
+      <c r="AX2" s="100"/>
+      <c r="AY2" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="AZ2" s="100"/>
-      <c r="BA2" s="99" t="s">
+      <c r="AZ2" s="102"/>
+      <c r="BA2" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="BB2" s="100"/>
-      <c r="BC2" s="99" t="s">
+      <c r="BB2" s="102"/>
+      <c r="BC2" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="BD2" s="100"/>
-      <c r="BE2" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BF2" s="98"/>
-      <c r="BG2" s="97"/>
-      <c r="BH2" s="98"/>
-      <c r="BI2" s="105" t="s">
+      <c r="BD2" s="102"/>
+      <c r="BE2" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF2" s="106"/>
+      <c r="BG2" s="105"/>
+      <c r="BH2" s="106"/>
+      <c r="BI2" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="BJ2" s="106"/>
-      <c r="BK2" s="99" t="s">
+      <c r="BJ2" s="110"/>
+      <c r="BK2" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="BL2" s="100"/>
-      <c r="BM2" s="99" t="s">
+      <c r="BL2" s="102"/>
+      <c r="BM2" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="BN2" s="100"/>
-      <c r="BO2" s="113" t="s">
+      <c r="BN2" s="102"/>
+      <c r="BO2" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="BP2" s="114"/>
-      <c r="BQ2" s="111" t="s">
+      <c r="BP2" s="100"/>
+      <c r="BQ2" s="114" t="s">
         <v>89</v>
       </c>
-      <c r="BR2" s="112"/>
-      <c r="BS2" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BT2" s="98"/>
+      <c r="BR2" s="115"/>
+      <c r="BS2" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BT2" s="106"/>
     </row>
     <row r="3" spans="1:72" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="119"/>
+      <c r="A3" s="98"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="12" t="s">
@@ -3117,8 +3117,8 @@
       <c r="O3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="110"/>
+      <c r="P3" s="112"/>
+      <c r="Q3" s="113"/>
       <c r="R3" s="3"/>
       <c r="S3" s="4" t="s">
         <v>36</v>
@@ -3272,17 +3272,17 @@
       </c>
     </row>
     <row r="4" spans="1:72" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="97"/>
-      <c r="C4" s="98"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="106"/>
       <c r="D4" s="103" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="104"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="98"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="106"/>
       <c r="H4" s="103" t="s">
         <v>59</v>
       </c>
@@ -3295,17 +3295,17 @@
         <v>0</v>
       </c>
       <c r="M4" s="104"/>
-      <c r="N4" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" s="98"/>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="115"/>
-      <c r="R4" s="98"/>
-      <c r="S4" s="105" t="s">
+      <c r="N4" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="106"/>
+      <c r="P4" s="105"/>
+      <c r="Q4" s="111"/>
+      <c r="R4" s="106"/>
+      <c r="S4" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="T4" s="106"/>
+      <c r="T4" s="110"/>
       <c r="U4" s="103" t="s">
         <v>62</v>
       </c>
@@ -3314,20 +3314,20 @@
         <v>63</v>
       </c>
       <c r="X4" s="104"/>
-      <c r="Y4" s="111" t="s">
+      <c r="Y4" s="114" t="s">
         <v>118</v>
       </c>
-      <c r="Z4" s="112"/>
+      <c r="Z4" s="115"/>
       <c r="AA4" s="103" t="s">
         <v>65</v>
       </c>
       <c r="AB4" s="104"/>
-      <c r="AC4" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="98"/>
-      <c r="AE4" s="97"/>
-      <c r="AF4" s="98"/>
+      <c r="AC4" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="106"/>
+      <c r="AE4" s="105"/>
+      <c r="AF4" s="106"/>
       <c r="AG4" s="107" t="s">
         <v>66</v>
       </c>
@@ -3336,10 +3336,10 @@
         <v>0</v>
       </c>
       <c r="AJ4" s="104"/>
-      <c r="AK4" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="98"/>
+      <c r="AK4" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="106"/>
       <c r="AM4" s="107" t="s">
         <v>67</v>
       </c>
@@ -3348,20 +3348,20 @@
         <v>59</v>
       </c>
       <c r="AP4" s="104"/>
-      <c r="AQ4" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="98"/>
-      <c r="AS4" s="97"/>
-      <c r="AT4" s="98"/>
+      <c r="AQ4" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="106"/>
+      <c r="AS4" s="105"/>
+      <c r="AT4" s="106"/>
       <c r="AU4" s="103" t="s">
         <v>58</v>
       </c>
       <c r="AV4" s="104"/>
-      <c r="AW4" s="111" t="s">
+      <c r="AW4" s="114" t="s">
         <v>86</v>
       </c>
-      <c r="AX4" s="112"/>
+      <c r="AX4" s="115"/>
       <c r="AY4" s="103" t="s">
         <v>65</v>
       </c>
@@ -3374,39 +3374,39 @@
         <v>63</v>
       </c>
       <c r="BD4" s="104"/>
-      <c r="BE4" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BF4" s="98"/>
-      <c r="BG4" s="97"/>
-      <c r="BH4" s="98"/>
-      <c r="BI4" s="105" t="s">
+      <c r="BE4" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF4" s="106"/>
+      <c r="BG4" s="105"/>
+      <c r="BH4" s="106"/>
+      <c r="BI4" s="109" t="s">
         <v>69</v>
       </c>
-      <c r="BJ4" s="106"/>
-      <c r="BK4" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL4" s="100"/>
+      <c r="BJ4" s="110"/>
+      <c r="BK4" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="102"/>
       <c r="BM4" s="103" t="s">
         <v>63</v>
       </c>
       <c r="BN4" s="104"/>
-      <c r="BO4" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BP4" s="98"/>
-      <c r="BQ4" s="111" t="s">
+      <c r="BO4" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP4" s="106"/>
+      <c r="BQ4" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="BR4" s="112"/>
-      <c r="BS4" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BT4" s="98"/>
+      <c r="BR4" s="115"/>
+      <c r="BS4" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BT4" s="106"/>
     </row>
     <row r="5" spans="1:72" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="119"/>
+      <c r="A5" s="98"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="12" t="s">
@@ -3445,8 +3445,8 @@
       <c r="O5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="109"/>
-      <c r="Q5" s="110"/>
+      <c r="P5" s="112"/>
+      <c r="Q5" s="113"/>
       <c r="R5" s="3"/>
       <c r="S5" s="2" t="s">
         <v>57</v>
@@ -3600,19 +3600,19 @@
       </c>
     </row>
     <row r="6" spans="1:72" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="119" t="s">
+      <c r="A6" s="98" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="98"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="106"/>
       <c r="D6" s="103" t="s">
         <v>74</v>
       </c>
       <c r="E6" s="104"/>
-      <c r="F6" s="111" t="s">
+      <c r="F6" s="114" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="112"/>
+      <c r="G6" s="115"/>
       <c r="H6" s="103" t="s">
         <v>0</v>
       </c>
@@ -3625,17 +3625,17 @@
         <v>77</v>
       </c>
       <c r="M6" s="104"/>
-      <c r="N6" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="O6" s="98"/>
-      <c r="P6" s="97"/>
-      <c r="Q6" s="115"/>
-      <c r="R6" s="98"/>
-      <c r="S6" s="105" t="s">
+      <c r="N6" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6" s="106"/>
+      <c r="P6" s="105"/>
+      <c r="Q6" s="111"/>
+      <c r="R6" s="106"/>
+      <c r="S6" s="109" t="s">
         <v>78</v>
       </c>
-      <c r="T6" s="106"/>
+      <c r="T6" s="110"/>
       <c r="U6" s="103" t="s">
         <v>79</v>
       </c>
@@ -3644,20 +3644,20 @@
         <v>80</v>
       </c>
       <c r="X6" s="104"/>
-      <c r="Y6" s="111" t="s">
+      <c r="Y6" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="Z6" s="112"/>
+      <c r="Z6" s="115"/>
       <c r="AA6" s="103" t="s">
         <v>82</v>
       </c>
       <c r="AB6" s="104"/>
-      <c r="AC6" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="98"/>
-      <c r="AE6" s="97"/>
-      <c r="AF6" s="98"/>
+      <c r="AC6" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="106"/>
+      <c r="AE6" s="105"/>
+      <c r="AF6" s="106"/>
       <c r="AG6" s="107" t="s">
         <v>83</v>
       </c>
@@ -3666,10 +3666,10 @@
         <v>77</v>
       </c>
       <c r="AJ6" s="104"/>
-      <c r="AK6" s="105" t="s">
+      <c r="AK6" s="109" t="s">
         <v>84</v>
       </c>
-      <c r="AL6" s="106"/>
+      <c r="AL6" s="110"/>
       <c r="AM6" s="107" t="s">
         <v>85</v>
       </c>
@@ -3678,20 +3678,20 @@
         <v>0</v>
       </c>
       <c r="AP6" s="104"/>
-      <c r="AQ6" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="98"/>
-      <c r="AS6" s="97"/>
-      <c r="AT6" s="98"/>
+      <c r="AQ6" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="106"/>
+      <c r="AS6" s="105"/>
+      <c r="AT6" s="106"/>
       <c r="AU6" s="103" t="s">
         <v>74</v>
       </c>
       <c r="AV6" s="104"/>
-      <c r="AW6" s="111" t="s">
+      <c r="AW6" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="AX6" s="112"/>
+      <c r="AX6" s="115"/>
       <c r="AY6" s="103" t="s">
         <v>82</v>
       </c>
@@ -3704,39 +3704,39 @@
         <v>80</v>
       </c>
       <c r="BD6" s="104"/>
-      <c r="BE6" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BF6" s="98"/>
-      <c r="BG6" s="97"/>
-      <c r="BH6" s="98"/>
-      <c r="BI6" s="105" t="s">
+      <c r="BE6" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF6" s="106"/>
+      <c r="BG6" s="105"/>
+      <c r="BH6" s="106"/>
+      <c r="BI6" s="109" t="s">
         <v>87</v>
       </c>
-      <c r="BJ6" s="106"/>
-      <c r="BK6" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL6" s="100"/>
+      <c r="BJ6" s="110"/>
+      <c r="BK6" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL6" s="102"/>
       <c r="BM6" s="103" t="s">
         <v>80</v>
       </c>
       <c r="BN6" s="104"/>
-      <c r="BO6" s="113" t="s">
+      <c r="BO6" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="BP6" s="114"/>
-      <c r="BQ6" s="111" t="s">
+      <c r="BP6" s="100"/>
+      <c r="BQ6" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="BR6" s="112"/>
-      <c r="BS6" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BT6" s="98"/>
+      <c r="BR6" s="115"/>
+      <c r="BS6" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BT6" s="106"/>
     </row>
     <row r="7" spans="1:72" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="119"/>
+      <c r="A7" s="98"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
       <c r="D7" s="12" t="s">
@@ -3775,8 +3775,8 @@
       <c r="O7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P7" s="109"/>
-      <c r="Q7" s="110"/>
+      <c r="P7" s="112"/>
+      <c r="Q7" s="113"/>
       <c r="R7" s="3"/>
       <c r="S7" s="2" t="s">
         <v>73</v>
@@ -3930,42 +3930,42 @@
       </c>
     </row>
     <row r="8" spans="1:72" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="119" t="s">
+      <c r="A8" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="97"/>
-      <c r="C8" s="98"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="103" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="104"/>
-      <c r="F8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="98"/>
+      <c r="F8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="106"/>
       <c r="H8" s="103" t="s">
         <v>0</v>
       </c>
       <c r="I8" s="104"/>
-      <c r="J8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" s="98"/>
+      <c r="J8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="106"/>
       <c r="L8" s="103" t="s">
         <v>0</v>
       </c>
       <c r="M8" s="104"/>
-      <c r="N8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="O8" s="98"/>
-      <c r="P8" s="97"/>
-      <c r="Q8" s="115"/>
-      <c r="R8" s="98"/>
-      <c r="S8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="T8" s="98"/>
+      <c r="N8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="O8" s="106"/>
+      <c r="P8" s="105"/>
+      <c r="Q8" s="111"/>
+      <c r="R8" s="106"/>
+      <c r="S8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="T8" s="106"/>
       <c r="U8" s="103" t="s">
         <v>0</v>
       </c>
@@ -3974,99 +3974,99 @@
         <v>0</v>
       </c>
       <c r="X8" s="104"/>
-      <c r="Y8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="98"/>
+      <c r="Y8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="106"/>
       <c r="AA8" s="103" t="s">
         <v>0</v>
       </c>
       <c r="AB8" s="104"/>
-      <c r="AC8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="98"/>
-      <c r="AE8" s="97"/>
-      <c r="AF8" s="98"/>
-      <c r="AG8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="98"/>
+      <c r="AC8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="106"/>
+      <c r="AE8" s="105"/>
+      <c r="AF8" s="106"/>
+      <c r="AG8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="106"/>
       <c r="AI8" s="103" t="s">
         <v>0</v>
       </c>
       <c r="AJ8" s="104"/>
-      <c r="AK8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="98"/>
-      <c r="AM8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="98"/>
+      <c r="AK8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="106"/>
+      <c r="AM8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="106"/>
       <c r="AO8" s="103" t="s">
         <v>0</v>
       </c>
       <c r="AP8" s="104"/>
-      <c r="AQ8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="98"/>
-      <c r="AS8" s="97"/>
-      <c r="AT8" s="98"/>
-      <c r="AU8" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV8" s="100"/>
-      <c r="AW8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="98"/>
-      <c r="AY8" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ8" s="100"/>
-      <c r="BA8" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="BB8" s="100"/>
-      <c r="BC8" s="99" t="s">
+      <c r="AQ8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="106"/>
+      <c r="AS8" s="105"/>
+      <c r="AT8" s="106"/>
+      <c r="AU8" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="102"/>
+      <c r="AW8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="106"/>
+      <c r="AY8" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="102"/>
+      <c r="BA8" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="102"/>
+      <c r="BC8" s="101" t="s">
         <v>93</v>
       </c>
-      <c r="BD8" s="100"/>
-      <c r="BE8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BF8" s="98"/>
-      <c r="BG8" s="97"/>
-      <c r="BH8" s="98"/>
-      <c r="BI8" s="105" t="s">
+      <c r="BD8" s="102"/>
+      <c r="BE8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="106"/>
+      <c r="BG8" s="105"/>
+      <c r="BH8" s="106"/>
+      <c r="BI8" s="109" t="s">
         <v>94</v>
       </c>
-      <c r="BJ8" s="106"/>
-      <c r="BK8" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL8" s="100"/>
-      <c r="BM8" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="BN8" s="100"/>
-      <c r="BO8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BP8" s="98"/>
-      <c r="BQ8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BR8" s="98"/>
-      <c r="BS8" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BT8" s="98"/>
+      <c r="BJ8" s="110"/>
+      <c r="BK8" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="102"/>
+      <c r="BM8" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN8" s="102"/>
+      <c r="BO8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP8" s="106"/>
+      <c r="BQ8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR8" s="106"/>
+      <c r="BS8" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BT8" s="106"/>
     </row>
     <row r="9" spans="1:72" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="119"/>
+      <c r="A9" s="98"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="D9" s="9" t="s">
@@ -4105,8 +4105,8 @@
       <c r="O9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P9" s="109"/>
-      <c r="Q9" s="110"/>
+      <c r="P9" s="112"/>
+      <c r="Q9" s="113"/>
       <c r="R9" s="3"/>
       <c r="S9" s="2" t="s">
         <v>0</v>
@@ -4260,143 +4260,143 @@
       </c>
     </row>
     <row r="10" spans="1:72" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="119" t="s">
+      <c r="A10" s="98" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="113"/>
-      <c r="C10" s="114"/>
-      <c r="D10" s="99" t="s">
+      <c r="B10" s="99"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="101" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="100"/>
-      <c r="F10" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="114"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="100"/>
       <c r="H10" s="103" t="s">
         <v>0</v>
       </c>
       <c r="I10" s="104"/>
-      <c r="J10" s="113" t="s">
+      <c r="J10" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="K10" s="114"/>
+      <c r="K10" s="100"/>
       <c r="L10" s="103" t="s">
         <v>99</v>
       </c>
       <c r="M10" s="104"/>
-      <c r="N10" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="O10" s="114"/>
-      <c r="P10" s="113"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="114"/>
-      <c r="S10" s="113" t="s">
+      <c r="N10" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="100"/>
+      <c r="P10" s="99"/>
+      <c r="Q10" s="118"/>
+      <c r="R10" s="100"/>
+      <c r="S10" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="T10" s="114"/>
-      <c r="U10" s="99" t="s">
+      <c r="T10" s="100"/>
+      <c r="U10" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="V10" s="100"/>
-      <c r="W10" s="99" t="s">
+      <c r="V10" s="102"/>
+      <c r="W10" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="X10" s="100"/>
-      <c r="Y10" s="113" t="s">
+      <c r="X10" s="102"/>
+      <c r="Y10" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="Z10" s="114"/>
+      <c r="Z10" s="100"/>
       <c r="AA10" s="103" t="s">
         <v>104</v>
       </c>
       <c r="AB10" s="104"/>
-      <c r="AC10" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="114"/>
-      <c r="AE10" s="113"/>
-      <c r="AF10" s="114"/>
-      <c r="AG10" s="113" t="s">
+      <c r="AC10" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="100"/>
+      <c r="AE10" s="99"/>
+      <c r="AF10" s="100"/>
+      <c r="AG10" s="99" t="s">
         <v>105</v>
       </c>
-      <c r="AH10" s="114"/>
+      <c r="AH10" s="100"/>
       <c r="AI10" s="103" t="s">
         <v>99</v>
       </c>
       <c r="AJ10" s="104"/>
-      <c r="AK10" s="113" t="s">
+      <c r="AK10" s="99" t="s">
         <v>106</v>
       </c>
-      <c r="AL10" s="114"/>
-      <c r="AM10" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN10" s="114"/>
+      <c r="AL10" s="100"/>
+      <c r="AM10" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="100"/>
       <c r="AO10" s="103" t="s">
         <v>0</v>
       </c>
       <c r="AP10" s="104"/>
-      <c r="AQ10" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="114"/>
-      <c r="AS10" s="113"/>
-      <c r="AT10" s="114"/>
-      <c r="AU10" s="99" t="s">
+      <c r="AQ10" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="100"/>
+      <c r="AS10" s="99"/>
+      <c r="AT10" s="100"/>
+      <c r="AU10" s="101" t="s">
         <v>97</v>
       </c>
-      <c r="AV10" s="100"/>
-      <c r="AW10" s="113" t="s">
+      <c r="AV10" s="102"/>
+      <c r="AW10" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="AX10" s="114"/>
-      <c r="AY10" s="99" t="s">
+      <c r="AX10" s="100"/>
+      <c r="AY10" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="AZ10" s="100"/>
-      <c r="BA10" s="99" t="s">
+      <c r="AZ10" s="102"/>
+      <c r="BA10" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="BB10" s="100"/>
-      <c r="BC10" s="99" t="s">
+      <c r="BB10" s="102"/>
+      <c r="BC10" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="BD10" s="100"/>
-      <c r="BE10" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="BF10" s="114"/>
-      <c r="BG10" s="113"/>
-      <c r="BH10" s="114"/>
-      <c r="BI10" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="BJ10" s="114"/>
-      <c r="BK10" s="99" t="s">
+      <c r="BD10" s="102"/>
+      <c r="BE10" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF10" s="100"/>
+      <c r="BG10" s="99"/>
+      <c r="BH10" s="100"/>
+      <c r="BI10" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="100"/>
+      <c r="BK10" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="BL10" s="100"/>
-      <c r="BM10" s="99" t="s">
+      <c r="BL10" s="102"/>
+      <c r="BM10" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="BN10" s="100"/>
-      <c r="BO10" s="113" t="s">
+      <c r="BN10" s="102"/>
+      <c r="BO10" s="99" t="s">
         <v>109</v>
       </c>
-      <c r="BP10" s="114"/>
-      <c r="BQ10" s="113" t="s">
+      <c r="BP10" s="100"/>
+      <c r="BQ10" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="BR10" s="114"/>
-      <c r="BS10" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="BT10" s="114"/>
+      <c r="BR10" s="100"/>
+      <c r="BS10" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="BT10" s="100"/>
     </row>
     <row r="11" spans="1:72" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="119"/>
+      <c r="A11" s="98"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="9" t="s">
@@ -4435,8 +4435,8 @@
       <c r="O11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P11" s="117"/>
-      <c r="Q11" s="118"/>
+      <c r="P11" s="116"/>
+      <c r="Q11" s="117"/>
       <c r="R11" s="5"/>
       <c r="S11" s="4" t="s">
         <v>96</v>
@@ -4590,19 +4590,19 @@
       </c>
     </row>
     <row r="12" spans="1:72" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="119" t="s">
+      <c r="A12" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="97"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="98"/>
-      <c r="F12" s="111" t="s">
+      <c r="B12" s="105"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="106"/>
+      <c r="F12" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="112"/>
+      <c r="G12" s="115"/>
       <c r="H12" s="103" t="s">
         <v>113</v>
       </c>
@@ -4615,55 +4615,55 @@
         <v>115</v>
       </c>
       <c r="M12" s="104"/>
-      <c r="N12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="O12" s="98"/>
-      <c r="P12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="115"/>
-      <c r="R12" s="98"/>
-      <c r="S12" s="105" t="s">
+      <c r="N12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="106"/>
+      <c r="P12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="111"/>
+      <c r="R12" s="106"/>
+      <c r="S12" s="109" t="s">
         <v>116</v>
       </c>
-      <c r="T12" s="106"/>
-      <c r="U12" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="V12" s="100"/>
-      <c r="W12" s="99" t="s">
+      <c r="T12" s="110"/>
+      <c r="U12" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="V12" s="102"/>
+      <c r="W12" s="101" t="s">
         <v>117</v>
       </c>
-      <c r="X12" s="100"/>
-      <c r="Y12" s="111" t="s">
+      <c r="X12" s="102"/>
+      <c r="Y12" s="114" t="s">
         <v>81</v>
       </c>
-      <c r="Z12" s="112"/>
-      <c r="AA12" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="100"/>
-      <c r="AC12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="98"/>
-      <c r="AE12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="98"/>
-      <c r="AG12" s="101" t="s">
+      <c r="Z12" s="115"/>
+      <c r="AA12" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="102"/>
+      <c r="AC12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="106"/>
+      <c r="AE12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="106"/>
+      <c r="AG12" s="119" t="s">
         <v>119</v>
       </c>
-      <c r="AH12" s="102"/>
+      <c r="AH12" s="120"/>
       <c r="AI12" s="103" t="s">
         <v>115</v>
       </c>
       <c r="AJ12" s="104"/>
-      <c r="AK12" s="105" t="s">
+      <c r="AK12" s="109" t="s">
         <v>120</v>
       </c>
-      <c r="AL12" s="106"/>
+      <c r="AL12" s="110"/>
       <c r="AM12" s="107" t="s">
         <v>121</v>
       </c>
@@ -4672,69 +4672,69 @@
         <v>113</v>
       </c>
       <c r="AP12" s="104"/>
-      <c r="AQ12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="98"/>
-      <c r="AS12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="98"/>
-      <c r="AU12" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="AV12" s="100"/>
-      <c r="AW12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="AX12" s="98"/>
-      <c r="AY12" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="AZ12" s="100"/>
-      <c r="BA12" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="BB12" s="100"/>
-      <c r="BC12" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="BD12" s="100"/>
-      <c r="BE12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BF12" s="98"/>
-      <c r="BG12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH12" s="98"/>
-      <c r="BI12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BJ12" s="98"/>
-      <c r="BK12" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="BL12" s="100"/>
-      <c r="BM12" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="BN12" s="100"/>
-      <c r="BO12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BP12" s="98"/>
-      <c r="BQ12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BR12" s="98"/>
-      <c r="BS12" s="97" t="s">
-        <v>0</v>
-      </c>
-      <c r="BT12" s="98"/>
+      <c r="AQ12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="106"/>
+      <c r="AS12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="106"/>
+      <c r="AU12" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV12" s="102"/>
+      <c r="AW12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX12" s="106"/>
+      <c r="AY12" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ12" s="102"/>
+      <c r="BA12" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB12" s="102"/>
+      <c r="BC12" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD12" s="102"/>
+      <c r="BE12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BF12" s="106"/>
+      <c r="BG12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH12" s="106"/>
+      <c r="BI12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BJ12" s="106"/>
+      <c r="BK12" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL12" s="102"/>
+      <c r="BM12" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN12" s="102"/>
+      <c r="BO12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP12" s="106"/>
+      <c r="BQ12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR12" s="106"/>
+      <c r="BS12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="BT12" s="106"/>
     </row>
     <row r="13" spans="1:72" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="119"/>
+      <c r="A13" s="98"/>
       <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
@@ -4777,10 +4777,10 @@
       <c r="O13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P13" s="109" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="110"/>
+      <c r="P13" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="113"/>
       <c r="R13" s="3" t="s">
         <v>0</v>
       </c>
@@ -4982,30 +4982,215 @@
     </row>
   </sheetData>
   <mergeCells count="257">
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="AU1:AV1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AY1:AZ1"/>
-    <mergeCell ref="BA1:BB1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="BO12:BP12"/>
+    <mergeCell ref="BQ12:BR12"/>
+    <mergeCell ref="BS12:BT12"/>
+    <mergeCell ref="BC12:BD12"/>
+    <mergeCell ref="BE12:BF12"/>
+    <mergeCell ref="BG12:BH12"/>
+    <mergeCell ref="BI12:BJ12"/>
+    <mergeCell ref="BK12:BL12"/>
+    <mergeCell ref="BM12:BN12"/>
+    <mergeCell ref="AQ12:AR12"/>
+    <mergeCell ref="AS12:AT12"/>
+    <mergeCell ref="AU12:AV12"/>
+    <mergeCell ref="AW12:AX12"/>
+    <mergeCell ref="AY12:AZ12"/>
+    <mergeCell ref="BA12:BB12"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AI12:AJ12"/>
+    <mergeCell ref="AK12:AL12"/>
+    <mergeCell ref="AM12:AN12"/>
+    <mergeCell ref="AO12:AP12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="BS10:BT10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="BG10:BH10"/>
+    <mergeCell ref="BI10:BJ10"/>
+    <mergeCell ref="BK10:BL10"/>
+    <mergeCell ref="BM10:BN10"/>
+    <mergeCell ref="BO10:BP10"/>
+    <mergeCell ref="BQ10:BR10"/>
+    <mergeCell ref="AU10:AV10"/>
+    <mergeCell ref="AW10:AX10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="AY10:AZ10"/>
+    <mergeCell ref="BA10:BB10"/>
+    <mergeCell ref="BC10:BD10"/>
+    <mergeCell ref="BE10:BF10"/>
+    <mergeCell ref="AI10:AJ10"/>
+    <mergeCell ref="AK10:AL10"/>
+    <mergeCell ref="AM10:AN10"/>
+    <mergeCell ref="AO10:AP10"/>
+    <mergeCell ref="AQ10:AR10"/>
+    <mergeCell ref="AS10:AT10"/>
+    <mergeCell ref="BM8:BN8"/>
+    <mergeCell ref="BO8:BP8"/>
+    <mergeCell ref="BQ8:BR8"/>
+    <mergeCell ref="BS8:BT8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="AY8:AZ8"/>
+    <mergeCell ref="BA8:BB8"/>
+    <mergeCell ref="BC8:BD8"/>
+    <mergeCell ref="BE8:BF8"/>
+    <mergeCell ref="BG8:BH8"/>
+    <mergeCell ref="BI8:BJ8"/>
+    <mergeCell ref="AM8:AN8"/>
+    <mergeCell ref="AO8:AP8"/>
+    <mergeCell ref="AQ8:AR8"/>
+    <mergeCell ref="AS8:AT8"/>
+    <mergeCell ref="AU8:AV8"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="AI8:AJ8"/>
+    <mergeCell ref="AK8:AL8"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="BK8:BL8"/>
+    <mergeCell ref="BQ2:BR2"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BE6:BF6"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="BI6:BJ6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BM6:BN6"/>
+    <mergeCell ref="AQ6:AR6"/>
+    <mergeCell ref="AS6:AT6"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AW8:AX8"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="AG8:AH8"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="BS4:BT4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="BK4:BL4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="BQ6:BR6"/>
+    <mergeCell ref="BQ4:BR4"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="BG4:BH4"/>
+    <mergeCell ref="BI4:BJ4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AW6:AX6"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="BE4:BF4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AO6:AP6"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="BS2:BT2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="AY2:AZ2"/>
+    <mergeCell ref="BA2:BB2"/>
+    <mergeCell ref="BC2:BD2"/>
+    <mergeCell ref="BE2:BF2"/>
+    <mergeCell ref="BG2:BH2"/>
+    <mergeCell ref="BI2:BJ2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="BK2:BL2"/>
+    <mergeCell ref="BM2:BN2"/>
+    <mergeCell ref="BO2:BP2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="S2:T2"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
@@ -5030,215 +5215,30 @@
     <mergeCell ref="BM1:BN1"/>
     <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="AS1:AT1"/>
-    <mergeCell ref="BS2:BT2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="AY2:AZ2"/>
-    <mergeCell ref="BA2:BB2"/>
-    <mergeCell ref="BC2:BD2"/>
-    <mergeCell ref="BE2:BF2"/>
-    <mergeCell ref="BG2:BH2"/>
-    <mergeCell ref="BI2:BJ2"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AQ2:AR2"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="BK2:BL2"/>
-    <mergeCell ref="BM2:BN2"/>
-    <mergeCell ref="BO2:BP2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AW2:AX2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="BG4:BH4"/>
-    <mergeCell ref="BI4:BJ4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AW6:AX6"/>
-    <mergeCell ref="AY4:AZ4"/>
-    <mergeCell ref="BA4:BB4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="BE4:BF4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AO6:AP6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="BS4:BT4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="BK4:BL4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="BO4:BP4"/>
-    <mergeCell ref="BQ6:BR6"/>
-    <mergeCell ref="BQ4:BR4"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="AG8:AH8"/>
-    <mergeCell ref="BQ2:BR2"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BE6:BF6"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="BI6:BJ6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BM6:BN6"/>
-    <mergeCell ref="AQ6:AR6"/>
-    <mergeCell ref="AS6:AT6"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AW8:AX8"/>
-    <mergeCell ref="AI8:AJ8"/>
-    <mergeCell ref="AK8:AL8"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="BK8:BL8"/>
-    <mergeCell ref="BM8:BN8"/>
-    <mergeCell ref="BO8:BP8"/>
-    <mergeCell ref="BQ8:BR8"/>
-    <mergeCell ref="BS8:BT8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="AY8:AZ8"/>
-    <mergeCell ref="BA8:BB8"/>
-    <mergeCell ref="BC8:BD8"/>
-    <mergeCell ref="BE8:BF8"/>
-    <mergeCell ref="BG8:BH8"/>
-    <mergeCell ref="BI8:BJ8"/>
-    <mergeCell ref="AM8:AN8"/>
-    <mergeCell ref="AO8:AP8"/>
-    <mergeCell ref="AQ8:AR8"/>
-    <mergeCell ref="AS8:AT8"/>
-    <mergeCell ref="AU8:AV8"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="AY10:AZ10"/>
-    <mergeCell ref="BA10:BB10"/>
-    <mergeCell ref="BC10:BD10"/>
-    <mergeCell ref="BE10:BF10"/>
-    <mergeCell ref="AI10:AJ10"/>
-    <mergeCell ref="AK10:AL10"/>
-    <mergeCell ref="AM10:AN10"/>
-    <mergeCell ref="AO10:AP10"/>
-    <mergeCell ref="AQ10:AR10"/>
-    <mergeCell ref="AS10:AT10"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="BS10:BT10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="BG10:BH10"/>
-    <mergeCell ref="BI10:BJ10"/>
-    <mergeCell ref="BK10:BL10"/>
-    <mergeCell ref="BM10:BN10"/>
-    <mergeCell ref="BO10:BP10"/>
-    <mergeCell ref="BQ10:BR10"/>
-    <mergeCell ref="AU10:AV10"/>
-    <mergeCell ref="AW10:AX10"/>
-    <mergeCell ref="AQ12:AR12"/>
-    <mergeCell ref="AS12:AT12"/>
-    <mergeCell ref="AU12:AV12"/>
-    <mergeCell ref="AW12:AX12"/>
-    <mergeCell ref="AY12:AZ12"/>
-    <mergeCell ref="BA12:BB12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="AK12:AL12"/>
-    <mergeCell ref="AM12:AN12"/>
-    <mergeCell ref="AO12:AP12"/>
-    <mergeCell ref="BO12:BP12"/>
-    <mergeCell ref="BQ12:BR12"/>
-    <mergeCell ref="BS12:BT12"/>
-    <mergeCell ref="BC12:BD12"/>
-    <mergeCell ref="BE12:BF12"/>
-    <mergeCell ref="BG12:BH12"/>
-    <mergeCell ref="BI12:BJ12"/>
-    <mergeCell ref="BK12:BL12"/>
-    <mergeCell ref="BM12:BN12"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AY1:AZ1"/>
+    <mergeCell ref="BA1:BB1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>